<commit_message>
animation loops fixed, and documentation of rTrachMan complete.
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 23 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 23 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FD068D-01A5-4A63-A37C-9E8CD149E3CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B17FDF-51FB-4A00-ABEE-8F2683F6EF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -530,8 +530,11 @@
       <c r="B13">
         <v>0.5</v>
       </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
       <c r="I13" s="1">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -545,10 +548,12 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="G14" s="1">
+        <v>3</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1">
-        <v>0.5</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
panels updated, inspect is a m mess.
</commit_message>
<xml_diff>
--- a/admin/Timesheets/Caroline Chang/Week 23 Timesheet.xlsx
+++ b/admin/Timesheets/Caroline Chang/Week 23 Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carol\CSCI_Classes\CSCI4308\capstone_proj\admin\Timesheets\Caroline Chang\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B17FDF-51FB-4A00-ABEE-8F2683F6EF2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B86B33D4-4083-4C10-8E2D-867DABC9FB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -427,7 +427,7 @@
   <dimension ref="A4:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K11" sqref="K10:K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -533,8 +533,11 @@
       <c r="G13">
         <v>3</v>
       </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
       <c r="I13" s="1">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -551,9 +554,11 @@
       <c r="G14" s="1">
         <v>3</v>
       </c>
-      <c r="H14" s="1"/>
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
       <c r="I14" s="1">
-        <v>3.5</v>
+        <v>6.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>